<commit_message>
FCAT_Ants data set complete. Ectatomman and Wasmannia entries completed. All formatted. Added .R file.
</commit_message>
<xml_diff>
--- a/Ants_students_data_july2023.xlsx
+++ b/Ants_students_data_july2023.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boloq\Box\Dissertation\FCAT\FCAT_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA28D264-7E98-45B6-9B42-B54990A010A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62DF6C1-C640-4A41-B29B-A1E6F60354E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{29C3B899-A9B4-4A5C-9A42-BD72ADC8363C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -540,7 +540,7 @@
   <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="A2" sqref="A2:L76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>